<commit_message>
Update 27. Previsão e Solver
Anotações e Prática. da Aula 8.
</commit_message>
<xml_diff>
--- a/27. Previsão e Solver/Previsão e Solver - Gerenciador de Cenários - Previsão e Solver - Pasta de Trabalho 3.xlsx
+++ b/27. Previsão e Solver/Previsão e Solver - Gerenciador de Cenários - Previsão e Solver - Pasta de Trabalho 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiko\Documents\Projetos Programação\Especializacao-em-Analise-de-Dados\27. Previsão e Solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144BDFC1-A587-4C7F-8738-E17DEE845784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226DBB1C-2FF0-4081-BBCD-23B9BA405E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" activeTab="1" xr2:uid="{25A05545-28B5-48BE-AB92-F3471190387D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" activeTab="3" xr2:uid="{25A05545-28B5-48BE-AB92-F3471190387D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cenários" sheetId="11" r:id="rId1"/>
@@ -1292,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E661F5B-44F2-43B6-9BF1-F362A1606875}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H2" sqref="G1:H2"/>
     </sheetView>
   </sheetViews>
@@ -1647,7 +1647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588CF6A4-1F1E-4CE5-82C3-8C9AFDA64599}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1938,7 +1940,10 @@
       <c r="G11" s="23">
         <v>8</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="20">
+        <f t="dataTable" ref="H11:H21" dt2D="0" dtr="0" r1="H2"/>
+        <v>36000</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -1963,7 +1968,9 @@
       <c r="G12" s="23">
         <v>9</v>
       </c>
-      <c r="H12" s="20"/>
+      <c r="H12" s="20">
+        <v>48000</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
@@ -1988,7 +1995,9 @@
       <c r="G13" s="23">
         <v>10</v>
       </c>
-      <c r="H13" s="20"/>
+      <c r="H13" s="20">
+        <v>60000</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -2009,49 +2018,65 @@
       <c r="G14" s="23">
         <v>11</v>
       </c>
-      <c r="H14" s="20"/>
+      <c r="H14" s="20">
+        <v>72000</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G15" s="23">
         <v>12</v>
       </c>
-      <c r="H15" s="20"/>
+      <c r="H15" s="20">
+        <v>84000</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" s="23">
         <v>13</v>
       </c>
-      <c r="H16" s="20"/>
+      <c r="H16" s="20">
+        <v>96000</v>
+      </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="23">
         <v>14</v>
       </c>
-      <c r="H17" s="20"/>
+      <c r="H17" s="20">
+        <v>108000</v>
+      </c>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="23">
         <v>15</v>
       </c>
-      <c r="H18" s="20"/>
+      <c r="H18" s="20">
+        <v>120000</v>
+      </c>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G19" s="23">
         <v>16</v>
       </c>
-      <c r="H19" s="20"/>
+      <c r="H19" s="20">
+        <v>132000</v>
+      </c>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G20" s="23">
         <v>17</v>
       </c>
-      <c r="H20" s="20"/>
+      <c r="H20" s="20">
+        <v>144000</v>
+      </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G21" s="23">
         <v>18</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="20">
+        <v>156000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2063,7 +2088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5509D2E2-1387-4784-8AF2-9370DB455379}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2336,10 +2363,19 @@
       <c r="G10" s="23">
         <v>8</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="H10" s="13">
+        <f t="dataTable" ref="H10:K20" dt2D="1" dtr="1" r1="H2" r2="H1"/>
+        <v>4000</v>
+      </c>
+      <c r="I10" s="13">
+        <v>20000</v>
+      </c>
+      <c r="J10" s="13">
+        <v>36000</v>
+      </c>
+      <c r="K10" s="13">
+        <v>52000</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -2364,10 +2400,18 @@
       <c r="G11" s="23">
         <v>9</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="H11" s="13">
+        <v>12000</v>
+      </c>
+      <c r="I11" s="13">
+        <v>30000</v>
+      </c>
+      <c r="J11" s="13">
+        <v>48000</v>
+      </c>
+      <c r="K11" s="13">
+        <v>66000</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -2392,10 +2436,18 @@
       <c r="G12" s="23">
         <v>10</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="H12" s="13">
+        <v>20000</v>
+      </c>
+      <c r="I12" s="13">
+        <v>40000</v>
+      </c>
+      <c r="J12" s="13">
+        <v>60000</v>
+      </c>
+      <c r="K12" s="13">
+        <v>80000</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
@@ -2420,10 +2472,18 @@
       <c r="G13" s="23">
         <v>11</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="H13" s="13">
+        <v>28000</v>
+      </c>
+      <c r="I13" s="13">
+        <v>50000</v>
+      </c>
+      <c r="J13" s="13">
+        <v>72000</v>
+      </c>
+      <c r="K13" s="13">
+        <v>94000</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -2444,64 +2504,120 @@
       <c r="G14" s="23">
         <v>12</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="H14" s="13">
+        <v>36000</v>
+      </c>
+      <c r="I14" s="13">
+        <v>60000</v>
+      </c>
+      <c r="J14" s="13">
+        <v>84000</v>
+      </c>
+      <c r="K14" s="13">
+        <v>108000</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G15" s="23">
         <v>13</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="H15" s="13">
+        <v>44000</v>
+      </c>
+      <c r="I15" s="13">
+        <v>70000</v>
+      </c>
+      <c r="J15" s="13">
+        <v>96000</v>
+      </c>
+      <c r="K15" s="13">
+        <v>122000</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G16" s="23">
         <v>14</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="H16" s="13">
+        <v>52000</v>
+      </c>
+      <c r="I16" s="13">
+        <v>80000</v>
+      </c>
+      <c r="J16" s="13">
+        <v>108000</v>
+      </c>
+      <c r="K16" s="13">
+        <v>136000</v>
+      </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G17" s="23">
         <v>15</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="H17" s="13">
+        <v>60000</v>
+      </c>
+      <c r="I17" s="13">
+        <v>90000</v>
+      </c>
+      <c r="J17" s="13">
+        <v>120000</v>
+      </c>
+      <c r="K17" s="13">
+        <v>150000</v>
+      </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G18" s="23">
         <v>16</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="H18" s="13">
+        <v>68000</v>
+      </c>
+      <c r="I18" s="13">
+        <v>100000</v>
+      </c>
+      <c r="J18" s="13">
+        <v>132000</v>
+      </c>
+      <c r="K18" s="13">
+        <v>164000</v>
+      </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G19" s="23">
         <v>17</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
+      <c r="H19" s="13">
+        <v>76000</v>
+      </c>
+      <c r="I19" s="13">
+        <v>110000</v>
+      </c>
+      <c r="J19" s="13">
+        <v>144000</v>
+      </c>
+      <c r="K19" s="13">
+        <v>178000</v>
+      </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G20" s="23">
         <v>18</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="H20" s="13">
+        <v>84000</v>
+      </c>
+      <c r="I20" s="13">
+        <v>120000</v>
+      </c>
+      <c r="J20" s="13">
+        <v>156000</v>
+      </c>
+      <c r="K20" s="13">
+        <v>192000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>